<commit_message>
Henderson experimental data added & working on clearance correction
</commit_message>
<xml_diff>
--- a/experimental_data/GEC/Henderson1982.xlsx
+++ b/experimental_data/GEC/Henderson1982.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="97">
   <si>
     <t>Henderson1982</t>
   </si>
@@ -288,6 +288,24 @@
   </si>
   <si>
     <t>GE</t>
+  </si>
+  <si>
+    <t>Table 2 – Galactose Clearance</t>
+  </si>
+  <si>
+    <t>Infusion rate [mg/min]</t>
+  </si>
+  <si>
+    <t>Infusion rate [mmole/min]</t>
+  </si>
+  <si>
+    <t>Clearance (steady state) [ml/min]</t>
+  </si>
+  <si>
+    <t>Steady state  galactose concentration [mmol/L]</t>
+  </si>
+  <si>
+    <t>Img</t>
   </si>
 </sst>
 </file>
@@ -529,15 +547,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>362880</xdr:colOff>
+      <xdr:colOff>389880</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>25560</xdr:rowOff>
+      <xdr:rowOff>16560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>522720</xdr:colOff>
+      <xdr:colOff>549360</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>18360</xdr:rowOff>
+      <xdr:rowOff>9000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -552,8 +570,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16550280" y="1492200"/>
-          <a:ext cx="9100440" cy="6864120"/>
+          <a:off x="16577280" y="1483200"/>
+          <a:ext cx="9100080" cy="6863760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -567,16 +585,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>296280</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>59040</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>587520</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>130320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>158040</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>90720</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>289440</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>62280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -591,8 +609,47 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="296280" y="10185120"/>
-          <a:ext cx="10359360" cy="1982520"/>
+          <a:off x="8556120" y="10419120"/>
+          <a:ext cx="10359000" cy="1982160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>141480</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>156600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1626840</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>143280</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 3" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1208880" y="12333240"/>
+          <a:ext cx="4310280" cy="3725640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -612,10 +669,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R56"/>
+  <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N47" activeCellId="0" sqref="N47:N56"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G85" activeCellId="0" sqref="G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3069,6 +3126,185 @@
         <v>0.387716666666667</v>
       </c>
     </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+    </row>
+    <row r="60" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <f aca="false">D62/180</f>
+        <v>0.277777777777778</v>
+      </c>
+      <c r="F62" s="0" t="n">
+        <v>1502</v>
+      </c>
+      <c r="G62" s="0" t="n">
+        <f aca="false">E62/F62*1000</f>
+        <v>0.184938600384672</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <f aca="false">D63/180</f>
+        <v>0.277777777777778</v>
+      </c>
+      <c r="F63" s="0" t="n">
+        <v>1572</v>
+      </c>
+      <c r="G63" s="0" t="n">
+        <f aca="false">E63/F63*1000</f>
+        <v>0.17670342097823</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <f aca="false">D64/180</f>
+        <v>0.255555555555556</v>
+      </c>
+      <c r="F64" s="0" t="n">
+        <v>1144</v>
+      </c>
+      <c r="G64" s="0" t="n">
+        <f aca="false">E64/F64*1000</f>
+        <v>0.223387723387723</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <f aca="false">D65/180</f>
+        <v>0.277777777777778</v>
+      </c>
+      <c r="F65" s="0" t="n">
+        <v>1333</v>
+      </c>
+      <c r="G65" s="0" t="n">
+        <f aca="false">E65/F65*1000</f>
+        <v>0.208385429690756</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B66" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <f aca="false">D66/180</f>
+        <v>0.338888888888889</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <v>1279</v>
+      </c>
+      <c r="G66" s="0" t="n">
+        <f aca="false">E66/F66*1000</f>
+        <v>0.264963947528451</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added clearance & GE correction for systematic galactose clearance
</commit_message>
<xml_diff>
--- a/experimental_data/GEC/Henderson1982.xlsx
+++ b/experimental_data/GEC/Henderson1982.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="98">
   <si>
     <t>Henderson1982</t>
   </si>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t>Steady state  galactose concentration [mmol/L]</t>
+  </si>
+  <si>
+    <t>Galactose elimination (CL*css) [mmol/min]</t>
   </si>
   <si>
     <t>Img</t>
@@ -585,16 +588,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>587520</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>403920</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>130320</xdr:rowOff>
+      <xdr:rowOff>95760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>289440</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>196560</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>62280</xdr:rowOff>
+      <xdr:rowOff>27720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -609,7 +612,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8556120" y="10419120"/>
+          <a:off x="9276120" y="10384560"/>
           <a:ext cx="10359000" cy="1982160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -671,8 +674,8 @@
   </sheetPr>
   <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G85" activeCellId="0" sqref="G85"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H63" activeCellId="0" sqref="H63:H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3156,6 +3159,9 @@
       <c r="G60" s="7" t="s">
         <v>95</v>
       </c>
+      <c r="H60" s="7" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="8" t="s">
@@ -3168,7 +3174,7 @@
         <v>15</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>51</v>
@@ -3178,6 +3184,9 @@
       </c>
       <c r="G61" s="8" t="s">
         <v>87</v>
+      </c>
+      <c r="H61" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3204,6 +3213,10 @@
         <f aca="false">E62/F62*1000</f>
         <v>0.184938600384672</v>
       </c>
+      <c r="H62" s="0" t="n">
+        <f aca="false">G62*F62/1000</f>
+        <v>0.277777777777778</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
@@ -3229,6 +3242,10 @@
         <f aca="false">E63/F63*1000</f>
         <v>0.17670342097823</v>
       </c>
+      <c r="H63" s="0" t="n">
+        <f aca="false">G63*F63/1000</f>
+        <v>0.277777777777778</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
@@ -3254,6 +3271,10 @@
         <f aca="false">E64/F64*1000</f>
         <v>0.223387723387723</v>
       </c>
+      <c r="H64" s="0" t="n">
+        <f aca="false">G64*F64/1000</f>
+        <v>0.255555555555556</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
@@ -3279,6 +3300,10 @@
         <f aca="false">E65/F65*1000</f>
         <v>0.208385429690756</v>
       </c>
+      <c r="H65" s="0" t="n">
+        <f aca="false">G65*F65/1000</f>
+        <v>0.277777777777778</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
@@ -3303,6 +3328,10 @@
       <c r="G66" s="0" t="n">
         <f aca="false">E66/F66*1000</f>
         <v>0.264963947528451</v>
+      </c>
+      <c r="H66" s="0" t="n">
+        <f aca="false">G66*F66/1000</f>
+        <v>0.338888888888889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>